<commit_message>
Added upper-bound exact comparision
</commit_message>
<xml_diff>
--- a/All_perf.xlsx
+++ b/All_perf.xlsx
@@ -1,42 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\workspaces\python\copt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttdkoc/Documents/dev/workspaces/python/copt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16578EC-9A16-4437-BE87-BC809C9A9959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C7FD77-504A-434D-839C-9C10A49B415F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{544C10BC-9448-4CAA-97CB-C174D9523FCA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" activeTab="1" xr2:uid="{544C10BC-9448-4CAA-97CB-C174D9523FCA}"/>
   </bookViews>
   <sheets>
     <sheet name="loose channel" sheetId="1" r:id="rId1"/>
     <sheet name="strict channel" sheetId="3" r:id="rId2"/>
-    <sheet name="Durations" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Durations" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Improved Greedy</t>
   </si>
@@ -61,6 +53,15 @@
   <si>
     <t>Basic Greedy</t>
   </si>
+  <si>
+    <t>UB</t>
+  </si>
+  <si>
+    <t>Gap %</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
 </sst>
 </file>
 
@@ -69,7 +70,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,8 +85,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,12 +106,93 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -112,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -122,9 +211,23 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -208,7 +311,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-TR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -801,7 +904,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1882279359"/>
@@ -860,7 +963,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1882278943"/>
@@ -902,7 +1005,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-TR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -939,7 +1042,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="tr-TR"/>
+      <a:endParaRPr lang="en-TR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1015,7 +1118,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-TR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1356,7 +1459,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1895933711"/>
@@ -1415,7 +1518,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1895935375"/>
@@ -1457,7 +1560,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-TR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1494,7 +1597,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="tr-TR"/>
+      <a:endParaRPr lang="en-TR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1575,7 +1678,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-TR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2076,7 +2179,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2001070095"/>
@@ -2135,7 +2238,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2001058863"/>
@@ -2177,7 +2280,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-TR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2214,7 +2317,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="tr-TR"/>
+      <a:endParaRPr lang="en-TR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2290,7 +2393,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-TR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3060,7 +3163,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="890864031"/>
@@ -3119,7 +3222,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="890857791"/>
@@ -3161,7 +3264,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-TR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3198,7 +3301,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="tr-TR"/>
+      <a:endParaRPr lang="en-TR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3274,7 +3377,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-TR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3949,7 +4052,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="247642127"/>
@@ -4008,7 +4111,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="247630063"/>
@@ -4050,7 +4153,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-TR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4087,7 +4190,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="tr-TR"/>
+      <a:endParaRPr lang="en-TR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4163,7 +4266,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-TR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4664,7 +4767,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1886368623"/>
@@ -4723,7 +4826,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1886370703"/>
@@ -4765,7 +4868,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-TR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4802,7 +4905,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="tr-TR"/>
+      <a:endParaRPr lang="en-TR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8194,16 +8297,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>98425</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>61912</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>328612</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>74612</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8230,16 +8333,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>300037</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>414337</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>136525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8679,51 +8782,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B31E84-D452-44EC-9AC7-099D3C0C767A}">
   <dimension ref="B1:R47"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="W36" sqref="W36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="3.140625" customWidth="1"/>
+    <col min="9" max="9" width="3.1640625" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" customWidth="1"/>
-    <col min="13" max="13" width="3.140625" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" customWidth="1"/>
-    <col min="16" max="16" width="3.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.5" customWidth="1"/>
+    <col min="13" max="13" width="3.1640625" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" customWidth="1"/>
+    <col min="16" max="16" width="3.1640625" customWidth="1"/>
     <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="J1" s="9" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="N1" s="9" t="s">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="N1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-    </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>1</v>
       </c>
@@ -8765,7 +8868,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>2</v>
       </c>
@@ -8807,7 +8910,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>3</v>
       </c>
@@ -8849,7 +8952,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>4</v>
       </c>
@@ -8891,7 +8994,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>5</v>
       </c>
@@ -8933,7 +9036,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>6</v>
       </c>
@@ -8975,7 +9078,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>7</v>
       </c>
@@ -9017,7 +9120,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>8</v>
       </c>
@@ -9059,7 +9162,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>9</v>
       </c>
@@ -9101,7 +9204,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>10</v>
       </c>
@@ -9143,7 +9246,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>11</v>
       </c>
@@ -9185,7 +9288,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>12</v>
       </c>
@@ -9227,7 +9330,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>13</v>
       </c>
@@ -9269,7 +9372,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>14</v>
       </c>
@@ -9311,7 +9414,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>15</v>
       </c>
@@ -9353,7 +9456,7 @@
       </c>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>16</v>
       </c>
@@ -9395,7 +9498,7 @@
       </c>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>17</v>
       </c>
@@ -9437,7 +9540,7 @@
       </c>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>18</v>
       </c>
@@ -9479,7 +9582,7 @@
       </c>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>19</v>
       </c>
@@ -9521,7 +9624,7 @@
       </c>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>20</v>
       </c>
@@ -9563,7 +9666,7 @@
       </c>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>21</v>
       </c>
@@ -9605,7 +9708,7 @@
       </c>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>22</v>
       </c>
@@ -9647,7 +9750,7 @@
       </c>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>23</v>
       </c>
@@ -9689,7 +9792,7 @@
       </c>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>24</v>
       </c>
@@ -9731,7 +9834,7 @@
       </c>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>25</v>
       </c>
@@ -9773,7 +9876,7 @@
       </c>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>26</v>
       </c>
@@ -9815,7 +9918,7 @@
       </c>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>27</v>
       </c>
@@ -9857,7 +9960,7 @@
       </c>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>28</v>
       </c>
@@ -9899,7 +10002,7 @@
       </c>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>29</v>
       </c>
@@ -9941,7 +10044,7 @@
       </c>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>30</v>
       </c>
@@ -9983,7 +10086,7 @@
       </c>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>31</v>
       </c>
@@ -10025,7 +10128,7 @@
       </c>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>32</v>
       </c>
@@ -10067,7 +10170,7 @@
       </c>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>33</v>
       </c>
@@ -10109,7 +10212,7 @@
       </c>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>34</v>
       </c>
@@ -10151,7 +10254,7 @@
       </c>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>35</v>
       </c>
@@ -10193,7 +10296,7 @@
       </c>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>36</v>
       </c>
@@ -10235,7 +10338,7 @@
       </c>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>37</v>
       </c>
@@ -10277,7 +10380,7 @@
       </c>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>38</v>
       </c>
@@ -10319,7 +10422,7 @@
       </c>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B40">
         <v>39</v>
       </c>
@@ -10361,7 +10464,7 @@
       </c>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>40</v>
       </c>
@@ -10403,7 +10506,7 @@
       </c>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>41</v>
       </c>
@@ -10445,7 +10548,7 @@
       </c>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>42</v>
       </c>
@@ -10487,7 +10590,7 @@
       </c>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>43</v>
       </c>
@@ -10529,7 +10632,7 @@
       </c>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>44</v>
       </c>
@@ -10571,7 +10674,7 @@
       </c>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>45</v>
       </c>
@@ -10613,7 +10716,7 @@
       </c>
       <c r="P46" s="1"/>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
       <c r="E47" s="1"/>
       <c r="I47" s="1"/>
       <c r="M47" s="1"/>
@@ -10641,45 +10744,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32456BF9-1A04-434C-AE1E-544544BF81F0}">
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G19" activeCellId="1" sqref="C19:C46 G19:G46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.140625" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.1640625" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="4.1640625" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="I1" s="9" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="I1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="M1" s="9" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="M1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="9"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N1" s="11"/>
+      <c r="P1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="11"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10719,10 +10827,20 @@
       <c r="N2">
         <v>90</v>
       </c>
-      <c r="Q2" s="5"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>90</v>
+      </c>
+      <c r="R2">
+        <f>(Q2-N2)/Q2</f>
+        <v>0</v>
+      </c>
       <c r="S2" s="5"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -10762,9 +10880,20 @@
       <c r="N3">
         <v>2604</v>
       </c>
-      <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O3" s="9"/>
+      <c r="P3" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>2604</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R19" si="3">(Q3-N3)/Q3</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="5"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -10804,9 +10933,20 @@
       <c r="N4">
         <v>5390</v>
       </c>
-      <c r="Q4" s="5"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O4" s="9"/>
+      <c r="P4" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>8300</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="3"/>
+        <v>0.35060240963855421</v>
+      </c>
+      <c r="S4" s="5"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -10846,9 +10986,20 @@
       <c r="N5">
         <v>7524</v>
       </c>
-      <c r="Q5" s="5"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O5" s="9"/>
+      <c r="P5" s="10">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>15048</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="S5" s="5"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -10888,9 +11039,20 @@
       <c r="N6">
         <v>8330</v>
       </c>
-      <c r="Q6" s="5"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O6" s="9"/>
+      <c r="P6" s="10">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>41650</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="S6" s="5"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -10930,9 +11092,20 @@
       <c r="N7">
         <v>33950</v>
       </c>
-      <c r="Q7" s="5"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O7" s="9"/>
+      <c r="P7" s="10">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>195700</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>0.82652018395503324</v>
+      </c>
+      <c r="S7" s="5"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -10972,9 +11145,20 @@
       <c r="N8">
         <v>20090</v>
       </c>
-      <c r="Q8" s="5"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O8" s="9"/>
+      <c r="P8" s="10">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>74664</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="3"/>
+        <v>0.73092789028179583</v>
+      </c>
+      <c r="S8" s="5"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11014,9 +11198,20 @@
       <c r="N9">
         <v>31200</v>
       </c>
-      <c r="Q9" s="5"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O9" s="9"/>
+      <c r="P9" s="10">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>270520</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>0.88466656809108379</v>
+      </c>
+      <c r="S9" s="5"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11056,9 +11251,20 @@
       <c r="N10">
         <v>54120</v>
       </c>
-      <c r="Q10" s="5"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O10" s="9"/>
+      <c r="P10" s="10">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>705516</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="3"/>
+        <v>0.92329018760736825</v>
+      </c>
+      <c r="S10" s="5"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11098,9 +11304,20 @@
       <c r="N11">
         <v>120540</v>
       </c>
-      <c r="Q11" s="5"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O11" s="9"/>
+      <c r="P11" s="10">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>1672862</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>0.92794384713144296</v>
+      </c>
+      <c r="S11" s="5"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11140,9 +11357,20 @@
       <c r="N12">
         <v>170720</v>
       </c>
-      <c r="Q12" s="5"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O12" s="9"/>
+      <c r="P12" s="10">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>1161046</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="3"/>
+        <v>0.85296017556582604</v>
+      </c>
+      <c r="S12" s="5"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11182,9 +11410,20 @@
       <c r="N13">
         <v>134550</v>
       </c>
-      <c r="Q13" s="5"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O13" s="9"/>
+      <c r="P13" s="10">
+        <v>12</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>1982340</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="3"/>
+        <v>0.93212566966312538</v>
+      </c>
+      <c r="S13" s="5"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11224,9 +11463,20 @@
       <c r="N14">
         <v>319600</v>
       </c>
-      <c r="Q14" s="5"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O14" s="9"/>
+      <c r="P14" s="10">
+        <v>13</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>4244663</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="3"/>
+        <v>0.92470544775875019</v>
+      </c>
+      <c r="S14" s="5"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11266,9 +11516,20 @@
       <c r="N15">
         <v>564000</v>
       </c>
-      <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O15" s="9"/>
+      <c r="P15" s="10">
+        <v>14</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>6378160</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="3"/>
+        <v>0.91157324369410608</v>
+      </c>
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11308,9 +11569,20 @@
       <c r="N16">
         <v>481600</v>
       </c>
-      <c r="Q16" s="5"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O16" s="9"/>
+      <c r="P16" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>4565882</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="3"/>
+        <v>0.89452202225112254</v>
+      </c>
+      <c r="S16" s="5"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11350,9 +11622,20 @@
       <c r="N17">
         <v>970000</v>
       </c>
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O17" s="9"/>
+      <c r="P17" s="10">
+        <v>16</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>14814516</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="3"/>
+        <v>0.93452367934261238</v>
+      </c>
+      <c r="S17" s="5"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11392,9 +11675,20 @@
       <c r="N18">
         <v>772200</v>
       </c>
-      <c r="Q18" s="5"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O18" s="9"/>
+      <c r="P18" s="10">
+        <v>17</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>11077403</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="3"/>
+        <v>0.93029052026002845</v>
+      </c>
+      <c r="S18" s="5"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -11423,15 +11717,17 @@
       <c r="J19" s="7"/>
       <c r="K19" s="4"/>
       <c r="L19" s="1"/>
-      <c r="M19">
+      <c r="M19" s="19">
         <v>18</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="19">
         <v>961450</v>
       </c>
+      <c r="O19" s="9"/>
+      <c r="P19" s="10"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -11466,10 +11762,11 @@
       <c r="N20">
         <v>1080400</v>
       </c>
+      <c r="O20" s="9"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="6"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -11504,11 +11801,12 @@
       <c r="N21">
         <v>1022753</v>
       </c>
+      <c r="O21" s="9"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="6"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -11543,10 +11841,11 @@
       <c r="N22">
         <v>2046126</v>
       </c>
+      <c r="O22" s="9"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -11581,10 +11880,11 @@
       <c r="N23">
         <v>3072344</v>
       </c>
+      <c r="O23" s="9"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -11619,10 +11919,11 @@
       <c r="N24">
         <v>4098271</v>
       </c>
+      <c r="O24" s="9"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="6"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -11657,10 +11958,11 @@
       <c r="N25">
         <v>5123100</v>
       </c>
+      <c r="O25" s="9"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -11695,10 +11997,11 @@
       <c r="N26">
         <v>6148618</v>
       </c>
+      <c r="O26" s="9"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -11733,10 +12036,11 @@
       <c r="N27">
         <v>7173833</v>
       </c>
+      <c r="O27" s="9"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -11771,10 +12075,11 @@
       <c r="N28">
         <v>8200514</v>
       </c>
+      <c r="O28" s="9"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -11809,10 +12114,11 @@
       <c r="N29">
         <v>9227822</v>
       </c>
+      <c r="O29" s="9"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="6"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -11847,10 +12153,11 @@
       <c r="N30">
         <v>10248345</v>
       </c>
+      <c r="O30" s="9"/>
       <c r="Q30" s="5"/>
       <c r="R30" s="6"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -11885,10 +12192,11 @@
       <c r="N31">
         <v>19760821</v>
       </c>
+      <c r="O31" s="9"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="6"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -11923,10 +12231,11 @@
       <c r="N32">
         <v>39543875</v>
       </c>
+      <c r="O32" s="9"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="6"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -11961,10 +12270,11 @@
       <c r="N33">
         <v>59325742</v>
       </c>
+      <c r="O33" s="9"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="6"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -11999,10 +12309,11 @@
       <c r="N34">
         <v>79082677</v>
       </c>
+      <c r="O34" s="9"/>
       <c r="Q34" s="5"/>
       <c r="R34" s="6"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -12037,10 +12348,11 @@
       <c r="N35">
         <v>98845051</v>
       </c>
+      <c r="O35" s="9"/>
       <c r="Q35" s="5"/>
       <c r="R35" s="6"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -12075,10 +12387,11 @@
       <c r="N36">
         <v>118617881</v>
       </c>
+      <c r="O36" s="9"/>
       <c r="Q36" s="5"/>
       <c r="R36" s="6"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -12113,10 +12426,11 @@
       <c r="N37">
         <v>138364819</v>
       </c>
+      <c r="O37" s="9"/>
       <c r="Q37" s="5"/>
       <c r="R37" s="6"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -12151,10 +12465,11 @@
       <c r="N38">
         <v>158100297</v>
       </c>
+      <c r="O38" s="9"/>
       <c r="Q38" s="5"/>
       <c r="R38" s="6"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -12189,10 +12504,11 @@
       <c r="N39">
         <v>177862585</v>
       </c>
+      <c r="O39" s="9"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="6"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -12227,10 +12543,11 @@
       <c r="N40">
         <v>197643615</v>
       </c>
+      <c r="O40" s="9"/>
       <c r="Q40" s="5"/>
       <c r="R40" s="6"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -12265,10 +12582,11 @@
       <c r="N41">
         <v>203391146</v>
       </c>
+      <c r="O41" s="9"/>
       <c r="Q41" s="5"/>
       <c r="R41" s="6"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -12303,10 +12621,11 @@
       <c r="N42">
         <v>237164680</v>
       </c>
+      <c r="O42" s="9"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="6"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -12341,10 +12660,11 @@
       <c r="N43">
         <v>256852145</v>
       </c>
+      <c r="O43" s="9"/>
       <c r="Q43" s="5"/>
       <c r="R43" s="6"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -12379,10 +12699,11 @@
       <c r="N44">
         <v>276772285</v>
       </c>
+      <c r="O44" s="9"/>
       <c r="Q44" s="5"/>
       <c r="R44" s="6"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -12417,10 +12738,11 @@
       <c r="N45">
         <v>296383891</v>
       </c>
+      <c r="O45" s="9"/>
       <c r="Q45" s="5"/>
       <c r="R45" s="6"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -12455,20 +12777,23 @@
       <c r="N46">
         <v>316232704</v>
       </c>
+      <c r="O46" s="9"/>
       <c r="Q46" s="5"/>
       <c r="R46" s="6"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="D47" s="1"/>
       <c r="H47" s="1"/>
       <c r="L47" s="1"/>
+      <c r="O47" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12481,27 +12806,200 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355891BB-3B71-4141-BEE4-80CDFF830844}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0.35060200000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15">
+        <v>0.82652000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15">
+        <v>0.73092800000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0.88466699999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="14">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15">
+        <v>0.92329000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="14">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0.92794399999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="14">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15">
+        <v>0.85296000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="14">
+        <v>12</v>
+      </c>
+      <c r="B13" s="15">
+        <v>0.93212600000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0.924705</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="14">
+        <v>14</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0.91157299999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="14">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0.89452200000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="14">
+        <v>16</v>
+      </c>
+      <c r="B17" s="15">
+        <v>0.93452400000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="16">
+        <v>17</v>
+      </c>
+      <c r="B18" s="17">
+        <v>0.93029099999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="18">
+        <f>AVERAGE(B6:B18)</f>
+        <v>0.88261923076923088</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C75FBA-F597-4FCA-8E75-147FEE67A9C3}">
   <dimension ref="B3:M48"/>
   <sheetViews>
-    <sheetView topLeftCell="H15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X39" sqref="X39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -12533,7 +13031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
@@ -12565,7 +13063,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>2</v>
       </c>
@@ -12597,7 +13095,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>3</v>
       </c>
@@ -12629,7 +13127,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>4</v>
       </c>
@@ -12661,7 +13159,7 @@
         <v>5.09</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>5</v>
       </c>
@@ -12693,7 +13191,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>6</v>
       </c>
@@ -12725,7 +13223,7 @@
         <v>16.739999999999998</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>7</v>
       </c>
@@ -12757,7 +13255,7 @@
         <v>27.34</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>8</v>
       </c>
@@ -12789,7 +13287,7 @@
         <v>56.73</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>9</v>
       </c>
@@ -12821,7 +13319,7 @@
         <v>106.88</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>10</v>
       </c>
@@ -12853,7 +13351,7 @@
         <v>183.1</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>11</v>
       </c>
@@ -12885,7 +13383,7 @@
         <v>219.84</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>12</v>
       </c>
@@ -12917,7 +13415,7 @@
         <v>238.67</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>13</v>
       </c>
@@ -12949,7 +13447,7 @@
         <v>476.17</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>14</v>
       </c>
@@ -12981,7 +13479,7 @@
         <v>821.61</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>15</v>
       </c>
@@ -13013,7 +13511,7 @@
         <v>1174.75</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>16</v>
       </c>
@@ -13045,7 +13543,7 @@
         <v>1400.85</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>17</v>
       </c>
@@ -13077,7 +13575,7 @@
         <v>1667.61</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>18</v>
       </c>
@@ -13107,7 +13605,7 @@
       </c>
       <c r="M21" s="5"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>19</v>
       </c>
@@ -13137,7 +13635,7 @@
       </c>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>20</v>
       </c>
@@ -13167,7 +13665,7 @@
       </c>
       <c r="M23" s="5"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>21</v>
       </c>
@@ -13197,7 +13695,7 @@
       </c>
       <c r="M24" s="5"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>22</v>
       </c>
@@ -13227,7 +13725,7 @@
       </c>
       <c r="M25" s="5"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>23</v>
       </c>
@@ -13257,7 +13755,7 @@
       </c>
       <c r="M26" s="5"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>24</v>
       </c>
@@ -13287,7 +13785,7 @@
       </c>
       <c r="M27" s="5"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>25</v>
       </c>
@@ -13317,7 +13815,7 @@
       </c>
       <c r="M28" s="5"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>26</v>
       </c>
@@ -13347,7 +13845,7 @@
       </c>
       <c r="M29" s="5"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>27</v>
       </c>
@@ -13377,7 +13875,7 @@
       </c>
       <c r="M30" s="5"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>28</v>
       </c>
@@ -13407,7 +13905,7 @@
       </c>
       <c r="M31" s="5"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>29</v>
       </c>
@@ -13437,7 +13935,7 @@
       </c>
       <c r="M32" s="5"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>30</v>
       </c>
@@ -13467,7 +13965,7 @@
       </c>
       <c r="M33" s="5"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>31</v>
       </c>
@@ -13497,7 +13995,7 @@
       </c>
       <c r="M34" s="5"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>32</v>
       </c>
@@ -13527,7 +14025,7 @@
       </c>
       <c r="M35" s="5"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>33</v>
       </c>
@@ -13557,7 +14055,7 @@
       </c>
       <c r="M36" s="5"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>34</v>
       </c>
@@ -13587,7 +14085,7 @@
       </c>
       <c r="M37" s="5"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>35</v>
       </c>
@@ -13617,7 +14115,7 @@
       </c>
       <c r="M38" s="5"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>36</v>
       </c>
@@ -13647,7 +14145,7 @@
       </c>
       <c r="M39" s="5"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B40">
         <v>37</v>
       </c>
@@ -13677,7 +14175,7 @@
       </c>
       <c r="M40" s="5"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>38</v>
       </c>
@@ -13707,7 +14205,7 @@
       </c>
       <c r="M41" s="5"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>39</v>
       </c>
@@ -13737,7 +14235,7 @@
       </c>
       <c r="M42" s="5"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>40</v>
       </c>
@@ -13767,7 +14265,7 @@
       </c>
       <c r="M43" s="5"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>41</v>
       </c>
@@ -13797,7 +14295,7 @@
       </c>
       <c r="M44" s="5"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>42</v>
       </c>
@@ -13827,7 +14325,7 @@
       </c>
       <c r="M45" s="5"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>43</v>
       </c>
@@ -13857,7 +14355,7 @@
       </c>
       <c r="M46" s="5"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B47">
         <v>44</v>
       </c>
@@ -13887,7 +14385,7 @@
       </c>
       <c r="M47" s="5"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B48">
         <v>45</v>
       </c>

</xml_diff>